<commit_message>
Complete updated paper -Pevi && -Clob
</commit_message>
<xml_diff>
--- a/supportFileProteins.xlsx
+++ b/supportFileProteins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="ComparisonTunicata" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,15 +19,18 @@
     <sheet name="Sheet7" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Sheet8" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Pivot Table_Sheet1_1" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="ComparisonTree" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Pivot Table_ComparisonTree_1" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId14"/>
-    <pivotCache cacheId="2" r:id="rId15"/>
-    <pivotCache cacheId="3" r:id="rId16"/>
-    <pivotCache cacheId="4" r:id="rId17"/>
-    <pivotCache cacheId="5" r:id="rId18"/>
-    <pivotCache cacheId="6" r:id="rId19"/>
+    <pivotCache cacheId="1" r:id="rId16"/>
+    <pivotCache cacheId="2" r:id="rId17"/>
+    <pivotCache cacheId="3" r:id="rId18"/>
+    <pivotCache cacheId="4" r:id="rId19"/>
+    <pivotCache cacheId="5" r:id="rId20"/>
+    <pivotCache cacheId="6" r:id="rId21"/>
+    <pivotCache cacheId="7" r:id="rId22"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="44">
   <si>
     <t xml:space="preserve">Specie</t>
   </si>
@@ -109,16 +112,13 @@
     <t xml:space="preserve">Average - %</t>
   </si>
   <si>
-    <t xml:space="preserve">Median - %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count - %</t>
-  </si>
-  <si>
     <t xml:space="preserve">StDev - %</t>
   </si>
   <si>
     <t xml:space="preserve">Total Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum - %</t>
   </si>
   <si>
     <t xml:space="preserve">P. miniata </t>
@@ -151,16 +151,36 @@
     <t xml:space="preserve">L. chalumnae </t>
   </si>
   <si>
-    <t xml:space="preserve">Sum - %</t>
+    <t xml:space="preserve">Sub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appendic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stolido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phlebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplouso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum - Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average - Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StDev - Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -206,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -323,6 +343,34 @@
       <left style="medium"/>
       <right style="thin"/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -403,27 +451,6 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -468,7 +495,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -525,7 +552,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,6 +576,26 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -561,75 +608,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="31" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="30" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,6 +683,114 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="8">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A27:E35" sheet="ComparisonTunicata"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Specie" numFmtId="0">
+      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="B. leachii "/>
+        <s v="B. schlosseri "/>
+        <s v="C. robusta "/>
+        <s v="C. savignyi "/>
+        <s v="D. vexillum "/>
+        <s v="M. occidentalis "/>
+        <s v="M. oculata "/>
+        <s v="O. dioica "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+        <n v="4565"/>
+        <n v="4808"/>
+        <n v="6846"/>
+        <n v="8167"/>
+        <n v="8428"/>
+        <n v="10206"/>
+        <n v="11209"/>
+        <n v="26966"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="%" numFmtId="0">
+      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+        <n v="14.72"/>
+        <n v="26.38"/>
+        <n v="27.93"/>
+        <n v="34.05"/>
+        <n v="39.66"/>
+        <n v="50.63"/>
+        <n v="51.29"/>
+        <n v="52.3"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Clade" numFmtId="0">
+      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="T"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Lifestyle" numFmtId="0">
+      <sharedItems count="2" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="C"/>
+        <s v="S"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="8">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A27:D35" sheet="ComparisonTunicata"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Specie" numFmtId="0">
+      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="B. leachii "/>
+        <s v="B. schlosseri "/>
+        <s v="C. robusta "/>
+        <s v="C. savignyi "/>
+        <s v="D. vexillum "/>
+        <s v="M. occidentalis "/>
+        <s v="M. oculata "/>
+        <s v="O. dioica "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+        <n v="4565"/>
+        <n v="4808"/>
+        <n v="6846"/>
+        <n v="8167"/>
+        <n v="8428"/>
+        <n v="10206"/>
+        <n v="11209"/>
+        <n v="26966"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="%" numFmtId="0">
+      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+        <n v="14.72"/>
+        <n v="26.38"/>
+        <n v="27.93"/>
+        <n v="34.05"/>
+        <n v="39.66"/>
+        <n v="50.63"/>
+        <n v="51.29"/>
+        <n v="52.3"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Clade" numFmtId="0">
+      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="T"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="8">
   <cacheSource type="worksheet">
     <worksheetSource ref="A15:E23" sheet="ComparisonTunicata"/>
@@ -708,7 +847,76 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="12">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:E13" sheet="ComparisonTunicata"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Specie" numFmtId="0">
+      <sharedItems count="12" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="B. leachii "/>
+        <s v="B. schlosseri "/>
+        <s v="C. oblonga (Ciro) "/>
+        <s v="C. oblonga (Oidi) "/>
+        <s v="C. robusta "/>
+        <s v="C. savignyi "/>
+        <s v="D. vexillum "/>
+        <s v="M. occidentalis "/>
+        <s v="M. oculata "/>
+        <s v="O. dioica "/>
+        <s v="P. viridis (Ciro) "/>
+        <s v="P. viridis (Oidi) "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems count="12" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+        <n v="1408"/>
+        <n v="1972"/>
+        <n v="1997"/>
+        <n v="2902"/>
+        <n v="4565"/>
+        <n v="4808"/>
+        <n v="6846"/>
+        <n v="8284"/>
+        <n v="8523"/>
+        <n v="10206"/>
+        <n v="11243"/>
+        <n v="28686"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="%" numFmtId="0">
+      <sharedItems count="12" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+        <n v="0.08"/>
+        <n v="0.09"/>
+        <n v="0.21"/>
+        <n v="0.25"/>
+        <n v="14.72"/>
+        <n v="26.38"/>
+        <n v="27.93"/>
+        <n v="34.05"/>
+        <n v="39.66"/>
+        <n v="50.63"/>
+        <n v="51.29"/>
+        <n v="52.3"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Clade" numFmtId="0">
+      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="T"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Life" numFmtId="0">
+      <sharedItems count="2" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="C"/>
+        <s v="S"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="19">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:D20" sheet="Sheet1"/>
@@ -796,76 +1004,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="12">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E13" sheet="ComparisonTunicata"/>
-  </cacheSource>
-  <cacheFields count="5">
-    <cacheField name="Specie" numFmtId="0">
-      <sharedItems count="12" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
-        <s v="B. leachii "/>
-        <s v="B. schlosseri "/>
-        <s v="C. oblonga (Ciro) "/>
-        <s v="C. oblonga (Oidi) "/>
-        <s v="C. robusta "/>
-        <s v="C. savignyi "/>
-        <s v="D. vexillum "/>
-        <s v="M. occidentalis "/>
-        <s v="M. oculata "/>
-        <s v="O. dioica "/>
-        <s v="P. viridis (Ciro) "/>
-        <s v="P. viridis (Oidi) "/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Total" numFmtId="0">
-      <sharedItems count="12" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="1356"/>
-        <n v="1900"/>
-        <n v="1966"/>
-        <n v="2838"/>
-        <n v="4565"/>
-        <n v="4808"/>
-        <n v="6846"/>
-        <n v="8167"/>
-        <n v="8428"/>
-        <n v="10206"/>
-        <n v="11209"/>
-        <n v="26966"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="%" numFmtId="0">
-      <sharedItems count="12" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="0.07"/>
-        <n v="0.09"/>
-        <n v="0.21"/>
-        <n v="0.24"/>
-        <n v="14.72"/>
-        <n v="26.38"/>
-        <n v="27.93"/>
-        <n v="33.94"/>
-        <n v="37.28"/>
-        <n v="50.63"/>
-        <n v="50.72"/>
-        <n v="51.56"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Clade" numFmtId="0">
-      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
-        <s v="T"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Life" numFmtId="0">
-      <sharedItems count="2" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
-        <s v="C"/>
-        <s v="S"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="15">
   <cacheSource type="worksheet">
     <worksheetSource ref="A22:D37" sheet="Sheet1"/>
@@ -941,61 +1080,10 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="8">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A27:D35" sheet="ComparisonTunicata"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Specie" numFmtId="0">
-      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
-        <s v="B. leachii "/>
-        <s v="B. schlosseri "/>
-        <s v="C. robusta "/>
-        <s v="C. savignyi "/>
-        <s v="D. vexillum "/>
-        <s v="M. occidentalis "/>
-        <s v="M. oculata "/>
-        <s v="O. dioica "/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Total" numFmtId="0">
-      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="4565"/>
-        <n v="4808"/>
-        <n v="6846"/>
-        <n v="8167"/>
-        <n v="8428"/>
-        <n v="10206"/>
-        <n v="11209"/>
-        <n v="26966"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="%" numFmtId="0">
-      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="14.72"/>
-        <n v="26.38"/>
-        <n v="27.93"/>
-        <n v="34.05"/>
-        <n v="39.66"/>
-        <n v="50.63"/>
-        <n v="51.29"/>
-        <n v="52.3"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Clade" numFmtId="0">
-      <sharedItems count="1" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
-        <s v="T"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="8">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A27:E35" sheet="ComparisonTunicata"/>
+    <worksheetSource ref="A1:E9" sheet="ComparisonTree"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Specie" numFmtId="0">
@@ -1012,26 +1100,14 @@
     </cacheField>
     <cacheField name="Total" numFmtId="0">
       <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="4565"/>
-        <n v="4808"/>
-        <n v="6846"/>
-        <n v="8167"/>
-        <n v="8428"/>
-        <n v="10206"/>
-        <n v="11209"/>
-        <n v="26966"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="%" numFmtId="0">
-      <sharedItems count="8" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="14.72"/>
-        <n v="26.38"/>
-        <n v="27.93"/>
-        <n v="34.05"/>
-        <n v="39.66"/>
-        <n v="50.63"/>
-        <n v="51.29"/>
-        <n v="52.3"/>
+        <n v="473"/>
+        <n v="661"/>
+        <n v="754"/>
+        <n v="763"/>
+        <n v="807"/>
+        <n v="879"/>
+        <n v="891"/>
+        <n v="1134"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Clade" numFmtId="0">
@@ -1045,6 +1121,14 @@
         <s v="S"/>
       </sharedItems>
     </cacheField>
+    <cacheField name="Sub" numFmtId="0">
+      <sharedItems count="4" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="1" containsNumber="0">
+        <s v="Aplouso"/>
+        <s v="Appendic"/>
+        <s v="Phlebo"/>
+        <s v="Stolido"/>
+      </sharedItems>
+    </cacheField>
   </cacheFields>
 </pivotCacheDefinition>
 </file>
@@ -1111,6 +1195,209 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="8">
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="8">
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="10"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="11"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="19">
   <r>
     <x v="14"/>
@@ -1229,96 +1516,7 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
-  <r>
-    <x v="9"/>
-    <x v="5"/>
-    <x v="6"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="10"/>
-    <x v="7"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <x v="8"/>
-    <x v="10"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="6"/>
-    <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="7"/>
-    <x v="11"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="4"/>
-    <x v="5"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="9"/>
-    <x v="9"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="11"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="11"/>
-    <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="15">
   <r>
     <x v="12"/>
@@ -1413,114 +1611,61 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="8">
   <r>
     <x v="7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="6"/>
+  </r>
+  <r>
     <x v="3"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="4"/>
-    <x v="6"/>
-    <x v="0"/>
-  </r>
-  <r>
+    <x v="2"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
     <x v="3"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="7"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="8">
-  <r>
-    <x v="7"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="6"/>
-    <x v="3"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="4"/>
-    <x v="6"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="7"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="7"/>
-    <x v="4"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
   </r>
@@ -1528,7 +1673,57 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
+  <location ref="A1:F6" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="4"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <dataFields count="4">
+    <dataField fld="2" subtotal="average"/>
+    <dataField fld="2" subtotal="stdDevp"/>
+    <dataField fld="2" subtotal="average"/>
+    <dataField fld="2" subtotal="average"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
+  <location ref="A1:E4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <dataFields count="4">
+    <dataField fld="2" subtotal="sum"/>
+    <dataField fld="2" subtotal="stdDevp"/>
+    <dataField fld="2" subtotal="sum"/>
+    <dataField fld="2" subtotal="sum"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
   <location ref="A1:E5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -1545,31 +1740,6 @@
   </colFields>
   <dataFields count="4">
     <dataField fld="2" subtotal="average"/>
-    <dataField fld="2" subtotal="count"/>
-    <dataField fld="2" subtotal="average"/>
-    <dataField fld="2" subtotal="average"/>
-  </dataFields>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
-  <location ref="A1:F8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <dataFields count="5">
-    <dataField fld="2" subtotal="average"/>
-    <dataField fld="2" subtotal="count"/>
     <dataField fld="2" subtotal="average"/>
     <dataField fld="2" subtotal="average"/>
     <dataField fld="2" subtotal="average"/>
@@ -1577,8 +1747,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
   <location ref="A1:D5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -1595,14 +1765,39 @@
   </colFields>
   <dataFields count="3">
     <dataField fld="2" subtotal="average"/>
-    <dataField fld="2" subtotal="count"/>
+    <dataField fld="2" subtotal="average"/>
     <dataField fld="2" subtotal="average"/>
   </dataFields>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot5" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
+  <location ref="A1:F8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <dataFields count="5">
+    <dataField fld="2" subtotal="sum"/>
+    <dataField fld="2" subtotal="stdDev"/>
+    <dataField fld="2" subtotal="sum"/>
+    <dataField fld="2" subtotal="sum"/>
+    <dataField fld="2" subtotal="sum"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
   <location ref="A1:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -1618,14 +1813,14 @@
   </colFields>
   <dataFields count="3">
     <dataField fld="2" subtotal="average"/>
-    <dataField fld="2" subtotal="count"/>
+    <dataField fld="2" subtotal="average"/>
     <dataField fld="2" subtotal="average"/>
   </dataFields>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
   <location ref="A1:F8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -1640,61 +1835,35 @@
     <field x="-2"/>
   </colFields>
   <dataFields count="5">
-    <dataField fld="2"/>
-    <dataField fld="2" subtotal="count"/>
     <dataField fld="2" subtotal="average"/>
-    <dataField fld="2" subtotal="sum"/>
-    <dataField fld="2" subtotal="stdDev"/>
+    <dataField fld="2" subtotal="average"/>
+    <dataField fld="2" subtotal="average"/>
+    <dataField fld="2" subtotal="average"/>
+    <dataField fld="2" subtotal="average"/>
   </dataFields>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot6" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
-  <location ref="A1:E4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="4">
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot8" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
+  <location ref="A1:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <dataFields count="4">
-    <dataField fld="2"/>
-    <dataField fld="2" subtotal="count"/>
-    <dataField fld="2" subtotal="average"/>
-    <dataField fld="2" subtotal="stdDevp"/>
-  </dataFields>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot7" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
-  <location ref="A1:F5" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="3"/>
     <field x="4"/>
   </rowFields>
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <dataFields count="4">
-    <dataField fld="2" subtotal="average"/>
-    <dataField fld="2"/>
-    <dataField fld="2" subtotal="count"/>
-    <dataField fld="2" subtotal="stdDevp"/>
+  <dataFields count="3">
+    <dataField fld="1" subtotal="sum"/>
+    <dataField fld="1" subtotal="average"/>
+    <dataField fld="1" subtotal="stdDev"/>
   </dataFields>
 </pivotTableDefinition>
 </file>
@@ -1706,8 +1875,8 @@
   </sheetPr>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27:E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2264,7 +2433,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A27:E35 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2287,170 +2456,170 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40" t="n">
+      <c r="B2" s="2" t="n">
         <v>4808</v>
       </c>
-      <c r="C2" s="40" t="n">
+      <c r="C2" s="2" t="n">
         <v>27.93</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="40" t="n">
+      <c r="B3" s="2" t="n">
         <v>11209</v>
       </c>
-      <c r="C3" s="40" t="n">
+      <c r="C3" s="2" t="n">
         <v>33.94</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="40" t="n">
+      <c r="B4" s="2" t="n">
         <v>8428</v>
       </c>
-      <c r="C4" s="40" t="n">
+      <c r="C4" s="2" t="n">
         <v>50.72</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="40" t="n">
+      <c r="B5" s="2" t="n">
         <v>6846</v>
       </c>
-      <c r="C5" s="40" t="n">
+      <c r="C5" s="2" t="n">
         <v>14.72</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="2" t="n">
         <v>8167</v>
       </c>
-      <c r="C6" s="40" t="n">
+      <c r="C6" s="2" t="n">
         <v>51.56</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="2" t="n">
         <v>4565</v>
       </c>
-      <c r="C7" s="40" t="n">
+      <c r="C7" s="2" t="n">
         <v>26.38</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="2" t="n">
         <v>10206</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="2" t="n">
         <v>50.63</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="40" t="n">
+      <c r="B9" s="2" t="n">
         <v>1900</v>
       </c>
-      <c r="C9" s="40" t="n">
+      <c r="C9" s="2" t="n">
         <v>0.09</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="40" t="n">
+      <c r="B10" s="2" t="n">
         <v>1356</v>
       </c>
-      <c r="C10" s="40" t="n">
+      <c r="C10" s="2" t="n">
         <v>0.07</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="40" t="n">
+      <c r="B11" s="2" t="n">
         <v>26966</v>
       </c>
-      <c r="C11" s="40" t="n">
+      <c r="C11" s="2" t="n">
         <v>37.28</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="40" t="n">
+      <c r="B12" s="2" t="n">
         <v>2838</v>
       </c>
-      <c r="C12" s="40" t="n">
+      <c r="C12" s="2" t="n">
         <v>0.24</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="40" t="n">
+      <c r="B13" s="2" t="n">
         <v>1966</v>
       </c>
-      <c r="C13" s="40" t="n">
+      <c r="C13" s="2" t="n">
         <v>0.21</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2473,7 +2642,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="A27:E35 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2482,7 +2651,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28"/>
+      <c r="A1" s="33"/>
       <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
@@ -2499,7 +2668,7 @@
         <v>22</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>22</v>
@@ -2519,7 +2688,7 @@
         <v>16.69</v>
       </c>
       <c r="C3" s="16" t="n">
-        <v>1</v>
+        <v>16.69</v>
       </c>
       <c r="D3" s="16" t="n">
         <v>16.69</v>
@@ -2532,103 +2701,405 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="35" t="n">
+      <c r="A4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="20" t="n">
         <v>56.105</v>
       </c>
-      <c r="C4" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="36" t="n">
+      <c r="C4" s="21" t="n">
         <v>56.105</v>
       </c>
-      <c r="E4" s="36" t="n">
+      <c r="D4" s="21" t="n">
         <v>56.105</v>
       </c>
-      <c r="F4" s="39" t="n">
+      <c r="E4" s="21" t="n">
         <v>56.105</v>
       </c>
+      <c r="F4" s="22" t="n">
+        <v>56.105</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="35" t="n">
+      <c r="A5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="20" t="n">
         <v>56.56</v>
       </c>
-      <c r="C5" s="36" t="n">
+      <c r="C5" s="21" t="n">
+        <v>56.56</v>
+      </c>
+      <c r="D5" s="21" t="n">
+        <v>56.56</v>
+      </c>
+      <c r="E5" s="21" t="n">
+        <v>56.56</v>
+      </c>
+      <c r="F5" s="22" t="n">
+        <v>56.56</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="20" t="n">
+        <v>24.7991666666667</v>
+      </c>
+      <c r="C6" s="21" t="n">
+        <v>24.7991666666667</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>24.7991666666667</v>
+      </c>
+      <c r="E6" s="21" t="n">
+        <v>24.7991666666667</v>
+      </c>
+      <c r="F6" s="22" t="n">
+        <v>24.7991666666667</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="25" t="n">
+        <v>51.71</v>
+      </c>
+      <c r="C7" s="26" t="n">
+        <v>51.71</v>
+      </c>
+      <c r="D7" s="26" t="n">
+        <v>51.71</v>
+      </c>
+      <c r="E7" s="26" t="n">
+        <v>51.71</v>
+      </c>
+      <c r="F7" s="27" t="n">
+        <v>51.71</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="30" t="n">
+        <v>33.5884210526316</v>
+      </c>
+      <c r="C8" s="31" t="n">
+        <v>33.5884210526316</v>
+      </c>
+      <c r="D8" s="31" t="n">
+        <v>33.5884210526316</v>
+      </c>
+      <c r="E8" s="31" t="n">
+        <v>33.5884210526316</v>
+      </c>
+      <c r="F8" s="32" t="n">
+        <v>33.5884210526316</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="36" t="n">
-        <v>56.56</v>
-      </c>
-      <c r="E5" s="36" t="n">
-        <v>56.56</v>
-      </c>
-      <c r="F5" s="39" t="n">
-        <v>56.56</v>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>473</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1134</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>879</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>891</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="35" t="n">
-        <v>24.7991666666667</v>
-      </c>
-      <c r="C6" s="36" t="n">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="36" t="n">
-        <v>24.7991666666667</v>
-      </c>
-      <c r="E6" s="36" t="n">
-        <v>24.7991666666667</v>
-      </c>
-      <c r="F6" s="39" t="n">
-        <v>24.7991666666667</v>
+      <c r="B6" s="0" t="n">
+        <v>661</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="20" t="n">
-        <v>51.71</v>
-      </c>
-      <c r="C7" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="21" t="n">
-        <v>51.71</v>
-      </c>
-      <c r="E7" s="21" t="n">
-        <v>51.71</v>
-      </c>
-      <c r="F7" s="22" t="n">
-        <v>51.71</v>
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>807</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="25" t="n">
-        <v>33.5884210526316</v>
-      </c>
-      <c r="C8" s="26" t="n">
-        <v>19</v>
-      </c>
-      <c r="D8" s="26" t="n">
-        <v>33.5884210526316</v>
-      </c>
-      <c r="E8" s="26" t="n">
-        <v>33.5884210526316</v>
-      </c>
-      <c r="F8" s="27" t="n">
-        <v>33.5884210526316</v>
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>754</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>763</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="33"/>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="15" t="n">
+        <v>763</v>
+      </c>
+      <c r="C3" s="16" t="n">
+        <v>763</v>
+      </c>
+      <c r="D3" s="40" t="e">
+        <f aca="false"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="20" t="n">
+        <v>473</v>
+      </c>
+      <c r="C4" s="21" t="n">
+        <v>473</v>
+      </c>
+      <c r="D4" s="41" t="e">
+        <f aca="false"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="20" t="n">
+        <v>1561</v>
+      </c>
+      <c r="C5" s="21" t="n">
+        <v>780.5</v>
+      </c>
+      <c r="D5" s="22" t="n">
+        <v>37.476659402887</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="25" t="n">
+        <v>3565</v>
+      </c>
+      <c r="C6" s="26" t="n">
+        <v>891.25</v>
+      </c>
+      <c r="D6" s="27" t="n">
+        <v>193.298344535074</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="30" t="n">
+        <v>6362</v>
+      </c>
+      <c r="C7" s="31" t="n">
+        <v>795.25</v>
+      </c>
+      <c r="D7" s="32" t="n">
+        <v>191.117577871395</v>
       </c>
     </row>
   </sheetData>
@@ -2647,10 +3118,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E45" activeCellId="1" sqref="A27:E35 E45"/>
+      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2682,66 +3153,82 @@
         <v>23</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>11</v>
-      </c>
+      <c r="B3" s="14"/>
       <c r="C3" s="15" t="n">
-        <v>35.56</v>
+        <v>37.12</v>
       </c>
       <c r="D3" s="16" t="n">
-        <v>39.66</v>
+        <v>12.8995232470041</v>
       </c>
       <c r="E3" s="16" t="n">
-        <v>3</v>
+        <v>37.12</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>15.613489893892</v>
+        <v>37.12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="20" t="n">
+        <v>35.56</v>
+      </c>
+      <c r="D4" s="21" t="n">
+        <v>15.613489893892</v>
+      </c>
+      <c r="E4" s="21" t="n">
+        <v>35.56</v>
+      </c>
+      <c r="F4" s="22" t="n">
+        <v>35.56</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="20" t="n">
+      <c r="C5" s="25" t="n">
         <v>38.056</v>
       </c>
-      <c r="D4" s="21" t="n">
-        <v>34.05</v>
-      </c>
-      <c r="E4" s="21" t="n">
-        <v>5</v>
-      </c>
-      <c r="F4" s="22" t="n">
+      <c r="D5" s="26" t="n">
         <v>10.8458021372326</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25" t="n">
+      <c r="E5" s="26" t="n">
+        <v>38.056</v>
+      </c>
+      <c r="F5" s="27" t="n">
+        <v>38.056</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30" t="n">
         <v>37.12</v>
       </c>
-      <c r="D5" s="26" t="n">
-        <v>36.855</v>
-      </c>
-      <c r="E5" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" s="27" t="n">
+      <c r="D6" s="31" t="n">
         <v>12.8995232470041</v>
+      </c>
+      <c r="E6" s="31" t="n">
+        <v>37.12</v>
+      </c>
+      <c r="F6" s="32" t="n">
+        <v>37.12</v>
       </c>
     </row>
   </sheetData>
@@ -2763,7 +3250,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="A27:E35 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2772,7 +3259,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28"/>
+      <c r="A1" s="33"/>
       <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
@@ -2785,13 +3272,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>25</v>
@@ -2801,34 +3288,34 @@
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="29" t="n">
-        <v>36.855</v>
-      </c>
-      <c r="C3" s="30" t="n">
-        <v>8</v>
-      </c>
-      <c r="D3" s="30" t="n">
-        <v>37.12</v>
-      </c>
-      <c r="E3" s="31" t="n">
+      <c r="B3" s="34" t="n">
+        <v>296.96</v>
+      </c>
+      <c r="C3" s="35" t="n">
         <v>12.8995232470041</v>
       </c>
+      <c r="D3" s="35" t="n">
+        <v>296.96</v>
+      </c>
+      <c r="E3" s="36" t="n">
+        <v>296.96</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="25" t="n">
-        <v>36.855</v>
-      </c>
-      <c r="C4" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="D4" s="26" t="n">
-        <v>37.12</v>
-      </c>
-      <c r="E4" s="27" t="n">
+      <c r="A4" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="30" t="n">
+        <v>296.96</v>
+      </c>
+      <c r="C4" s="31" t="n">
         <v>12.8995232470041</v>
+      </c>
+      <c r="D4" s="31" t="n">
+        <v>296.96</v>
+      </c>
+      <c r="E4" s="32" t="n">
+        <v>296.96</v>
       </c>
     </row>
   </sheetData>
@@ -2850,7 +3337,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="A27:E35 D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2859,7 +3346,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28"/>
+      <c r="A1" s="33"/>
       <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
@@ -2875,7 +3362,7 @@
         <v>22</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>22</v>
@@ -2892,7 +3379,7 @@
         <v>34.52</v>
       </c>
       <c r="C3" s="16" t="n">
-        <v>3</v>
+        <v>34.52</v>
       </c>
       <c r="D3" s="16" t="n">
         <v>34.52</v>
@@ -2902,36 +3389,36 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="20" t="n">
+      <c r="B4" s="25" t="n">
         <v>37.92</v>
       </c>
-      <c r="C4" s="21" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="21" t="n">
+      <c r="C4" s="26" t="n">
         <v>37.92</v>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="D4" s="26" t="n">
         <v>37.92</v>
       </c>
+      <c r="E4" s="27" t="n">
+        <v>37.92</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="25" t="n">
+      <c r="A5" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="30" t="n">
         <v>36.645</v>
       </c>
-      <c r="C5" s="26" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" s="26" t="n">
+      <c r="C5" s="31" t="n">
         <v>36.645</v>
       </c>
-      <c r="E5" s="27" t="n">
+      <c r="D5" s="31" t="n">
+        <v>36.645</v>
+      </c>
+      <c r="E5" s="32" t="n">
         <v>36.645</v>
       </c>
     </row>
@@ -2954,7 +3441,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A27:E35 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2963,7 +3450,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28"/>
+      <c r="A1" s="33"/>
       <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
@@ -2978,7 +3465,7 @@
         <v>22</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>22</v>
@@ -2989,41 +3476,41 @@
         <v>11</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>14.8814285714286</v>
+        <v>15.33</v>
       </c>
       <c r="C3" s="16" t="n">
+        <v>15.33</v>
+      </c>
+      <c r="D3" s="17" t="n">
+        <v>15.33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="17" t="n">
-        <v>14.8814285714286</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="20" t="n">
-        <v>37.92</v>
-      </c>
-      <c r="C4" s="21" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="22" t="n">
-        <v>37.92</v>
+      <c r="B4" s="25" t="n">
+        <v>38.056</v>
+      </c>
+      <c r="C4" s="26" t="n">
+        <v>38.056</v>
+      </c>
+      <c r="D4" s="27" t="n">
+        <v>38.056</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="25" t="n">
-        <v>24.4808333333333</v>
-      </c>
-      <c r="C5" s="26" t="n">
-        <v>12</v>
-      </c>
-      <c r="D5" s="27" t="n">
-        <v>24.4808333333333</v>
+      <c r="A5" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="30" t="n">
+        <v>24.7991666666667</v>
+      </c>
+      <c r="C5" s="31" t="n">
+        <v>24.7991666666667</v>
+      </c>
+      <c r="D5" s="32" t="n">
+        <v>24.7991666666667</v>
       </c>
     </row>
   </sheetData>
@@ -3045,7 +3532,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A27:E35 A1"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3072,7 +3559,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>15927</v>
@@ -3081,12 +3568,12 @@
         <v>56.42</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>12631</v>
@@ -3095,12 +3582,12 @@
         <v>55.79</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>9137</v>
@@ -3109,12 +3596,12 @@
         <v>56.56</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>8480</v>
@@ -3296,7 +3783,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>6072</v>
@@ -3305,12 +3792,12 @@
         <v>53.06</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>23892</v>
@@ -3319,12 +3806,12 @@
         <v>53.7</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>11416</v>
@@ -3333,7 +3820,7 @@
         <v>48.37</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3352,7 +3839,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>15927</v>
@@ -3361,12 +3848,12 @@
         <v>52.39</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>12631</v>
@@ -3375,12 +3862,12 @@
         <v>35.3</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>9137</v>
@@ -3389,12 +3876,12 @@
         <v>41.32</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>8480</v>
@@ -3520,7 +4007,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6072</v>
@@ -3529,12 +4016,12 @@
         <v>53.06</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>23892</v>
@@ -3543,12 +4030,12 @@
         <v>53.7</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>11416</v>
@@ -3557,7 +4044,7 @@
         <v>48.37</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3579,7 +4066,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="A27:E35 C24"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3590,7 +4077,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28"/>
+      <c r="A1" s="33"/>
       <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
@@ -3604,16 +4091,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>25</v>
@@ -3626,8 +4113,9 @@
       <c r="B3" s="15" t="n">
         <v>16.69</v>
       </c>
-      <c r="C3" s="16" t="n">
-        <v>1</v>
+      <c r="C3" s="38" t="e">
+        <f aca="false"/>
+        <v>#VALUE!</v>
       </c>
       <c r="D3" s="16" t="n">
         <v>16.69</v>
@@ -3635,110 +4123,109 @@
       <c r="E3" s="16" t="n">
         <v>16.69</v>
       </c>
-      <c r="F3" s="34" t="e">
+      <c r="F3" s="17" t="n">
+        <v>16.69</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="20" t="n">
+        <v>112.21</v>
+      </c>
+      <c r="C4" s="21" t="n">
+        <v>0.445477272146354</v>
+      </c>
+      <c r="D4" s="21" t="n">
+        <v>112.21</v>
+      </c>
+      <c r="E4" s="21" t="n">
+        <v>112.21</v>
+      </c>
+      <c r="F4" s="22" t="n">
+        <v>112.21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="20" t="n">
+        <v>56.56</v>
+      </c>
+      <c r="C5" s="39" t="e">
         <f aca="false"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="35" t="n">
-        <v>56.105</v>
-      </c>
-      <c r="C4" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="36" t="n">
-        <v>56.105</v>
-      </c>
-      <c r="E4" s="36" t="n">
-        <v>112.21</v>
-      </c>
-      <c r="F4" s="37" t="n">
-        <v>0.445477272146354</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="35" t="n">
+      <c r="D5" s="21" t="n">
         <v>56.56</v>
       </c>
-      <c r="C5" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="36" t="n">
+      <c r="E5" s="21" t="n">
         <v>56.56</v>
       </c>
-      <c r="E5" s="36" t="n">
+      <c r="F5" s="22" t="n">
         <v>56.56</v>
       </c>
-      <c r="F5" s="38" t="e">
-        <f aca="false"/>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="35" t="n">
-        <v>27.155</v>
-      </c>
-      <c r="C6" s="36" t="n">
-        <v>12</v>
-      </c>
-      <c r="D6" s="36" t="n">
-        <v>24.7991666666667</v>
-      </c>
-      <c r="E6" s="36" t="n">
+      <c r="A6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="20" t="n">
         <v>297.59</v>
       </c>
-      <c r="F6" s="39" t="n">
+      <c r="C6" s="21" t="n">
         <v>21.2655801529708</v>
       </c>
+      <c r="D6" s="21" t="n">
+        <v>297.59</v>
+      </c>
+      <c r="E6" s="21" t="n">
+        <v>297.59</v>
+      </c>
+      <c r="F6" s="22" t="n">
+        <v>297.59</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="20" t="n">
-        <v>53.06</v>
-      </c>
-      <c r="C7" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="21" t="n">
-        <v>51.71</v>
-      </c>
-      <c r="E7" s="21" t="n">
+      <c r="A7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="25" t="n">
         <v>155.13</v>
       </c>
-      <c r="F7" s="22" t="n">
+      <c r="C7" s="26" t="n">
         <v>2.91017181623366</v>
       </c>
+      <c r="D7" s="26" t="n">
+        <v>155.13</v>
+      </c>
+      <c r="E7" s="26" t="n">
+        <v>155.13</v>
+      </c>
+      <c r="F7" s="27" t="n">
+        <v>155.13</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="25" t="n">
-        <v>39.66</v>
-      </c>
-      <c r="C8" s="26" t="n">
-        <v>19</v>
-      </c>
-      <c r="D8" s="26" t="n">
-        <v>33.5884210526316</v>
-      </c>
-      <c r="E8" s="26" t="n">
+      <c r="A8" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="30" t="n">
         <v>638.18</v>
       </c>
-      <c r="F8" s="27" t="n">
+      <c r="C8" s="31" t="n">
         <v>22.0240273497323</v>
+      </c>
+      <c r="D8" s="31" t="n">
+        <v>638.18</v>
+      </c>
+      <c r="E8" s="31" t="n">
+        <v>638.18</v>
+      </c>
+      <c r="F8" s="32" t="n">
+        <v>638.18</v>
       </c>
     </row>
   </sheetData>
@@ -3760,7 +4247,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A27:E35 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3769,7 +4256,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28"/>
+      <c r="A1" s="33"/>
       <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
@@ -3784,7 +4271,7 @@
         <v>22</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>22</v>
@@ -3792,85 +4279,85 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B3" s="15" t="n">
+        <v>16.69</v>
+      </c>
+      <c r="C3" s="16" t="n">
+        <v>16.69</v>
+      </c>
+      <c r="D3" s="17" t="n">
+        <v>16.69</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="20" t="n">
+        <v>43.845</v>
+      </c>
+      <c r="C4" s="21" t="n">
+        <v>43.845</v>
+      </c>
+      <c r="D4" s="22" t="n">
+        <v>43.845</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="20" t="n">
+        <v>41.32</v>
+      </c>
+      <c r="C5" s="21" t="n">
+        <v>41.32</v>
+      </c>
+      <c r="D5" s="22" t="n">
+        <v>41.32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="20" t="n">
+        <v>36.645</v>
+      </c>
+      <c r="C6" s="21" t="n">
+        <v>36.645</v>
+      </c>
+      <c r="D6" s="22" t="n">
+        <v>36.645</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="25" t="n">
         <v>51.71</v>
       </c>
-      <c r="C3" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="17" t="n">
+      <c r="C7" s="26" t="n">
         <v>51.71</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="35" t="n">
-        <v>36.645</v>
-      </c>
-      <c r="C4" s="36" t="n">
-        <v>8</v>
-      </c>
-      <c r="D4" s="39" t="n">
-        <v>36.645</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="35" t="n">
-        <v>41.32</v>
-      </c>
-      <c r="C5" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="39" t="n">
-        <v>41.32</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="35" t="n">
-        <v>43.845</v>
-      </c>
-      <c r="C6" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="39" t="n">
-        <v>43.845</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="20" t="n">
-        <v>16.69</v>
-      </c>
-      <c r="C7" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="22" t="n">
-        <v>16.69</v>
+      <c r="D7" s="27" t="n">
+        <v>51.71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="25" t="n">
+      <c r="A8" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="30" t="n">
         <v>39.5993333333333</v>
       </c>
-      <c r="C8" s="26" t="n">
-        <v>15</v>
-      </c>
-      <c r="D8" s="27" t="n">
+      <c r="C8" s="31" t="n">
+        <v>39.5993333333333</v>
+      </c>
+      <c r="D8" s="32" t="n">
         <v>39.5993333333333</v>
       </c>
     </row>
@@ -3893,7 +4380,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="A27:E35 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3916,45 +4403,45 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>6072</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>53.06</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="40" t="n">
-        <v>6072</v>
-      </c>
-      <c r="C2" s="40" t="n">
-        <v>53.06</v>
-      </c>
-      <c r="D2" s="40" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40" t="s">
+      <c r="B3" s="2" t="n">
+        <v>23892</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="40" t="n">
-        <v>23892</v>
-      </c>
-      <c r="C3" s="40" t="n">
-        <v>53.7</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="40" t="n">
+      <c r="B4" s="2" t="n">
         <v>11416</v>
       </c>
-      <c r="C4" s="40" t="n">
+      <c r="C4" s="2" t="n">
         <v>48.37</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>34</v>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>